<commit_message>
Added table to P2
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mormi170899\Programmering\Webtek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikal\Documents\Webtex\Prohect\it2805gruppe31\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93395FDB-3C92-4CD6-8893-B170038350D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16820" windowHeight="7760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -164,7 +165,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,19 +478,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -503,7 +504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -518,7 +519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -532,7 +533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -546,7 +547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>12</v>
       </c>
@@ -560,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -575,7 +576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -589,7 +590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -603,7 +604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>14</v>
       </c>
@@ -617,7 +618,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>16</v>
       </c>
@@ -631,7 +632,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>15</v>
       </c>
@@ -645,7 +646,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>27</v>
       </c>
@@ -662,7 +663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>29</v>
       </c>
@@ -679,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>30</v>
       </c>
@@ -693,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>31</v>
       </c>
@@ -707,7 +708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>36</v>
       </c>
@@ -721,7 +722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>39</v>
       </c>
@@ -735,7 +736,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>40</v>
       </c>
@@ -749,7 +750,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.35">
       <c r="L22" s="2"/>
     </row>
   </sheetData>

</xml_diff>